<commit_message>
update back bearings pillow blocks
</commit_message>
<xml_diff>
--- a/calcs/RC Car Calcs.xlsx
+++ b/calcs/RC Car Calcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darren\Documents\Solidworks\RC_Car\calcs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darre\Documents\Personal Files\Solidworks\Car\calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FF6F4E-D3E8-4A4E-9ED9-E5732BD7C21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8D8606-C79F-46D0-8832-7ECF33973D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="1" xr2:uid="{852037FD-E437-4CF4-89D0-BA178B4F63EC}"/>
+    <workbookView xWindow="21840" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{852037FD-E437-4CF4-89D0-BA178B4F63EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts List" sheetId="2" r:id="rId1"/>
@@ -347,9 +347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -387,7 +387,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -493,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -635,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -649,9 +649,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -659,7 +659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -667,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -675,7 +675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -683,12 +683,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -696,7 +696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
@@ -719,20 +719,20 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.06640625" customWidth="1"/>
+    <col min="1" max="1" width="12.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -740,7 +740,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -751,7 +751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -759,7 +759,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -768,29 +768,29 @@
         <v>247.8136977848101</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -816,14 +816,14 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="3"/>
+    <col min="1" max="1" width="13.61328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.69140625" customWidth="1"/>
+    <col min="3" max="3" width="9.07421875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -834,7 +834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -845,7 +845,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -859,7 +859,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -870,7 +870,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -881,7 +881,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -892,7 +892,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>22</v>
       </c>

</xml_diff>